<commit_message>
Test 2 share ke linga
</commit_message>
<xml_diff>
--- a/Data testing Excel/Parameter Credit review.xlsx
+++ b/Data testing Excel/Parameter Credit review.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="41">
   <si>
     <t>Use</t>
   </si>
@@ -119,7 +119,25 @@
     <t>Edit Customer</t>
   </si>
   <si>
-    <t>539APP20240300343</t>
+    <t>Jamin</t>
+  </si>
+  <si>
+    <t>Mobil</t>
+  </si>
+  <si>
+    <t>Mycash</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>539APP20240500398</t>
+  </si>
+  <si>
+    <t>539APP20240500399</t>
+  </si>
+  <si>
+    <t>539APP20240600414</t>
   </si>
 </sst>
 </file>
@@ -477,17 +495,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
@@ -495,9 +513,10 @@
     <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,13 +547,16 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -560,12 +582,17 @@
       <c r="J2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C3" t="s">
         <v>22</v>
       </c>
@@ -590,10 +617,48 @@
       <c r="J3" t="s">
         <v>19</v>
       </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -604,17 +669,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.36328125" customWidth="1"/>
     <col min="2" max="2" width="21.7265625" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
@@ -622,7 +687,7 @@
     <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,14 +712,18 @@
       <c r="H1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>'Credit Review'!A2</f>
+        <v>Yes</v>
       </c>
       <c r="B2" t="str">
         <f>'Credit Review'!B2</f>
-        <v>539APP20240300343</v>
+        <v>539APP20240600414</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -668,14 +737,17 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="str">
         <f>'Credit Review'!B2</f>
-        <v>539APP20240300343</v>
+        <v>539APP20240600414</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -691,14 +763,17 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="str">
         <f>'Credit Review'!B2</f>
-        <v>539APP20240300343</v>
+        <v>539APP20240600414</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -716,14 +791,18 @@
       <c r="H4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>'Credit Review'!A3</f>
+        <v>No</v>
+      </c>
+      <c r="B5" t="str">
         <f>'Credit Review'!B3</f>
-        <v>0</v>
+        <v>539APP20240500399</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -737,14 +816,17 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
         <f>'Credit Review'!B3</f>
-        <v>0</v>
+        <v>539APP20240500399</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -760,14 +842,17 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
         <f>'Credit Review'!B3</f>
-        <v>0</v>
+        <v>539APP20240500399</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -785,21 +870,103 @@
       <c r="H7" t="s">
         <v>33</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>'Credit Review'!A4</f>
+        <v>No</v>
+      </c>
+      <c r="B8" t="str">
+        <f>'Credit Review'!B4</f>
+        <v>539APP20240500398</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="str">
+        <f>'Credit Review'!B4</f>
+        <v>539APP20240500398</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="str">
+        <f>'Credit Review'!B4</f>
+        <v>539APP20240500398</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations disablePrompts="1" count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F6">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F6 F9">
       <formula1>"Bad Character,Indikasi Fraud"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 H7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 H7 H10">
       <formula1>"Edit Application,Edit Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+      <formula1>"Approve,Reject,Return"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A10">
       <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
-      <formula1>"Approve,Reject,Return"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>